<commit_message>
deleted a bunch of files?
</commit_message>
<xml_diff>
--- a/data/2019PredsB.xlsx
+++ b/data/2019PredsB.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tang-\Documents\Python\skynet2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BABDE48-B3BD-4491-9AD7-EB4A175BDA8B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{614BD566-83F9-4807-8D86-A9861F1552ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4155" uniqueCount="589">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4162" uniqueCount="596">
   <si>
     <t>divsRank</t>
   </si>
@@ -1802,6 +1802,27 @@
   <si>
     <t>Count of swimmerName</t>
   </si>
+  <si>
+    <t>Actual</t>
+  </si>
+  <si>
+    <t>Trad error</t>
+  </si>
+  <si>
+    <t>GBR error</t>
+  </si>
+  <si>
+    <t>Abs trad error</t>
+  </si>
+  <si>
+    <t>Abs GBR error</t>
+  </si>
+  <si>
+    <t>MSE Trad</t>
+  </si>
+  <si>
+    <t>MSE GBR</t>
+  </si>
 </sst>
 </file>
 
@@ -2284,7 +2305,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2292,6 +2313,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -18489,7 +18512,7 @@
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField axis="axisRow" showAll="0" sortType="descending">
+    <pivotField axis="axisRow" showAll="0" sortType="ascending">
       <items count="32">
         <item x="22"/>
         <item x="7"/>
@@ -18524,15 +18547,6 @@
         <item x="16"/>
         <item t="default"/>
       </items>
-      <autoSortScope>
-        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
-          <references count="1">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </autoSortScope>
     </pivotField>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
@@ -19044,25 +19058,52 @@
   </rowFields>
   <rowItems count="32">
     <i>
-      <x v="28"/>
+      <x/>
     </i>
     <i>
-      <x v="22"/>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
     </i>
     <i>
       <x v="11"/>
     </i>
     <i>
-      <x/>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="14"/>
     </i>
     <i>
       <x v="15"/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="18"/>
     </i>
     <i>
       <x v="16"/>
@@ -19071,19 +19112,19 @@
       <x v="17"/>
     </i>
     <i>
-      <x v="5"/>
+      <x v="18"/>
     </i>
     <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="2"/>
+      <x v="19"/>
     </i>
     <i>
       <x v="20"/>
     </i>
     <i>
-      <x v="29"/>
+      <x v="21"/>
+    </i>
+    <i>
+      <x v="22"/>
     </i>
     <i>
       <x v="23"/>
@@ -19092,49 +19133,22 @@
       <x v="24"/>
     </i>
     <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="12"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="14"/>
-    </i>
-    <i>
       <x v="25"/>
     </i>
     <i>
-      <x v="19"/>
+      <x v="26"/>
     </i>
     <i>
       <x v="27"/>
     </i>
     <i>
-      <x v="30"/>
+      <x v="28"/>
     </i>
     <i>
-      <x v="3"/>
+      <x v="29"/>
     </i>
     <i>
-      <x v="26"/>
-    </i>
-    <i>
-      <x v="21"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="7"/>
+      <x v="30"/>
     </i>
     <i t="grand">
       <x/>
@@ -19476,10 +19490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:M40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19490,7 +19504,7 @@
     <col min="4" max="4" width="21.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -19498,7 +19512,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
@@ -19506,7 +19520,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
@@ -19514,7 +19528,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -19522,7 +19536,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
@@ -19530,7 +19544,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
@@ -19538,7 +19552,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>585</v>
       </c>
@@ -19551,442 +19565,1301 @@
       <c r="D8" t="s">
         <v>588</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F8" t="s">
+        <v>589</v>
+      </c>
+      <c r="G8" t="s">
+        <v>590</v>
+      </c>
+      <c r="H8" t="s">
+        <v>591</v>
+      </c>
+      <c r="I8" t="s">
+        <v>592</v>
+      </c>
+      <c r="J8" t="s">
+        <v>593</v>
+      </c>
+      <c r="K8" t="s">
+        <v>594</v>
+      </c>
+      <c r="L8" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B9" s="2">
+        <v>531</v>
+      </c>
+      <c r="C9" s="2">
+        <v>516.25975403563223</v>
+      </c>
+      <c r="D9" s="2">
+        <v>46</v>
+      </c>
+      <c r="F9">
+        <v>535</v>
+      </c>
+      <c r="G9">
+        <f>F9-GETPIVOTDATA("Sum of tradPred",$A$8,"school",A9)</f>
+        <v>4</v>
+      </c>
+      <c r="H9">
+        <f>F9-GETPIVOTDATA("Sum of gbrPred",$A$8,"school",A9)</f>
+        <v>18.740245964367773</v>
+      </c>
+      <c r="I9">
+        <f>ABS(G9)</f>
+        <v>4</v>
+      </c>
+      <c r="J9">
+        <f>ABS(H9)</f>
+        <v>18.740245964367773</v>
+      </c>
+      <c r="K9">
+        <f>G9^2</f>
+        <v>16</v>
+      </c>
+      <c r="L9">
+        <f>H9^2</f>
+        <v>351.19681880500258</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="2">
+        <v>465</v>
+      </c>
+      <c r="C10" s="2">
+        <v>448.35445200174451</v>
+      </c>
+      <c r="D10" s="2">
+        <v>53</v>
+      </c>
+      <c r="F10">
+        <v>447</v>
+      </c>
+      <c r="G10">
+        <f t="shared" ref="G10:G39" si="0">F10-GETPIVOTDATA("Sum of tradPred",$A$8,"school",A10)</f>
+        <v>-18</v>
+      </c>
+      <c r="H10">
+        <f t="shared" ref="H10:H39" si="1">F10-GETPIVOTDATA("Sum of gbrPred",$A$8,"school",A10)</f>
+        <v>-1.3544520017445052</v>
+      </c>
+      <c r="I10">
+        <f t="shared" ref="I10:J39" si="2">ABS(G10)</f>
+        <v>18</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="2"/>
+        <v>1.3544520017445052</v>
+      </c>
+      <c r="K10">
+        <f t="shared" ref="K10:K39" si="3">G10^2</f>
+        <v>324</v>
+      </c>
+      <c r="L10">
+        <f t="shared" ref="L10:L39" si="4">H10^2</f>
+        <v>1.8345402250296972</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="2">
+        <v>302</v>
+      </c>
+      <c r="C11" s="2">
+        <v>284.34660060496839</v>
+      </c>
+      <c r="D11" s="2">
+        <v>32</v>
+      </c>
+      <c r="F11">
+        <v>319</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B9" s="2">
+      <c r="H11">
+        <f t="shared" si="1"/>
+        <v>34.653399395031613</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="2"/>
+        <v>34.653399395031613</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="3"/>
+        <v>289</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="4"/>
+        <v>1200.8580896315773</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B12" s="2">
+        <v>28</v>
+      </c>
+      <c r="C12" s="2">
+        <v>25.6571923240163</v>
+      </c>
+      <c r="D12" s="2">
+        <v>2</v>
+      </c>
+      <c r="F12">
+        <v>27</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="1"/>
+        <v>1.3428076759836998</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="2"/>
+        <v>1.3428076759836998</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="4"/>
+        <v>1.8031324546807448</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B13" s="2">
+        <v>121</v>
+      </c>
+      <c r="C13" s="2">
+        <v>123.42551760010409</v>
+      </c>
+      <c r="D13" s="2">
+        <v>20</v>
+      </c>
+      <c r="F13">
+        <v>105</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>-16</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>-18.425517600104087</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="2"/>
+        <v>18.425517600104087</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="3"/>
+        <v>256</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="4"/>
+        <v>339.49969883174543</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="2">
+        <v>362</v>
+      </c>
+      <c r="C14" s="2">
+        <v>352.16573369588434</v>
+      </c>
+      <c r="D14" s="2">
+        <v>38</v>
+      </c>
+      <c r="F14">
+        <v>350</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>-12</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="1"/>
+        <v>-2.1657336958843416</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="2"/>
+        <v>2.1657336958843416</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="3"/>
+        <v>144</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="4"/>
+        <v>4.6904024414888497</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" s="2">
+        <v>13</v>
+      </c>
+      <c r="C15" s="2">
+        <v>13.015605521714182</v>
+      </c>
+      <c r="D15" s="2">
+        <v>3</v>
+      </c>
+      <c r="F15">
+        <v>12</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="1"/>
+        <v>-1.0156055217141819</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="2"/>
+        <v>1.0156055217141819</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="4"/>
+        <v>1.0314545757363356</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="B16" s="2">
+        <v>0</v>
+      </c>
+      <c r="C16" s="2">
+        <v>-0.33896476365591793</v>
+      </c>
+      <c r="D16" s="2">
+        <v>2</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="1"/>
+        <v>0.33896476365591793</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="2"/>
+        <v>0.33896476365591793</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="4"/>
+        <v>0.1148971110003123</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="2">
+        <v>317</v>
+      </c>
+      <c r="C17" s="2">
+        <v>307.85536265728939</v>
+      </c>
+      <c r="D17" s="2">
+        <v>34</v>
+      </c>
+      <c r="F17">
+        <v>294</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="0"/>
+        <v>-23</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="1"/>
+        <v>-13.85536265728939</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="2"/>
+        <v>13.85536265728939</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="3"/>
+        <v>529</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="4"/>
+        <v>191.97107436500931</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="B18" s="2">
+        <v>88</v>
+      </c>
+      <c r="C18" s="2">
+        <v>87.099190755294501</v>
+      </c>
+      <c r="D18" s="2">
+        <v>13</v>
+      </c>
+      <c r="F18">
+        <v>87</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="1"/>
+        <v>-9.9190755294500832E-2</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="2"/>
+        <v>9.9190755294500832E-2</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="4"/>
+        <v>9.838805935893544E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>440</v>
+      </c>
+      <c r="B19" s="2">
+        <v>0</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0.58402094684819805</v>
+      </c>
+      <c r="D19" s="2">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="1"/>
+        <v>-0.58402094684819805</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="2"/>
+        <v>0.58402094684819805</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="4"/>
+        <v>0.34108046635746575</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="2">
+        <v>606</v>
+      </c>
+      <c r="C20" s="2">
+        <v>595.33152670653919</v>
+      </c>
+      <c r="D20" s="2">
+        <v>58</v>
+      </c>
+      <c r="F20">
+        <v>591</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="0"/>
+        <v>-15</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="1"/>
+        <v>-4.3315267065391936</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="2"/>
+        <v>4.3315267065391936</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="3"/>
+        <v>225</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="4"/>
+        <v>18.762123609462272</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="2">
+        <v>107</v>
+      </c>
+      <c r="C21" s="2">
+        <v>103.96810032766695</v>
+      </c>
+      <c r="D21" s="2">
+        <v>12</v>
+      </c>
+      <c r="F21">
+        <v>97</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="0"/>
+        <v>-10</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="1"/>
+        <v>-6.9681003276669458</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="2"/>
+        <v>6.9681003276669458</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="4"/>
+        <v>48.554422176432197</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B22" s="2">
+        <v>11</v>
+      </c>
+      <c r="C22" s="2">
+        <v>11.03313150360686</v>
+      </c>
+      <c r="D22" s="2">
+        <v>2</v>
+      </c>
+      <c r="F22">
+        <v>7</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="1"/>
+        <v>-4.0331315036068602</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="2"/>
+        <v>4.0331315036068602</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="4"/>
+        <v>16.266149725386132</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B23" s="2">
+        <v>79</v>
+      </c>
+      <c r="C23" s="2">
+        <v>75.485696418629317</v>
+      </c>
+      <c r="D23" s="2">
+        <v>9</v>
+      </c>
+      <c r="F23">
+        <v>91</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="1"/>
+        <v>15.514303581370683</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="2"/>
+        <v>15.514303581370683</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="3"/>
+        <v>144</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="4"/>
+        <v>240.69361561493119</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B24" s="2">
+        <v>505</v>
+      </c>
+      <c r="C24" s="2">
+        <v>492.0426102315655</v>
+      </c>
+      <c r="D24" s="2">
+        <v>58</v>
+      </c>
+      <c r="F24">
+        <v>530</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="1"/>
+        <v>37.957389768434496</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="2"/>
+        <v>37.957389768434496</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="3"/>
+        <v>625</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="4"/>
+        <v>1440.7634380328557</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="2">
+        <v>418</v>
+      </c>
+      <c r="C25" s="2">
+        <v>406.60459841848473</v>
+      </c>
+      <c r="D25" s="2">
+        <v>31</v>
+      </c>
+      <c r="F25">
+        <v>405</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="0"/>
+        <v>-13</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="1"/>
+        <v>-1.6045984184847271</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="2"/>
+        <v>1.6045984184847271</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="3"/>
+        <v>169</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="4"/>
+        <v>2.5747360846036873</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B26" s="2">
+        <v>409</v>
+      </c>
+      <c r="C26" s="2">
+        <v>393.43649479845675</v>
+      </c>
+      <c r="D26" s="2">
+        <v>30</v>
+      </c>
+      <c r="F26">
+        <v>385</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="0"/>
+        <v>-24</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="1"/>
+        <v>-8.4364947984567493</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="2"/>
+        <v>8.4364947984567493</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="3"/>
+        <v>576</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="4"/>
+        <v>71.174444484387791</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B27" s="2">
+        <v>442</v>
+      </c>
+      <c r="C27" s="2">
+        <v>431.65038303467304</v>
+      </c>
+      <c r="D27" s="2">
+        <v>49</v>
+      </c>
+      <c r="F27">
+        <v>449</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="1"/>
+        <v>17.349616965326959</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="2"/>
+        <v>17.349616965326959</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="3"/>
+        <v>49</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="4"/>
+        <v>301.00920884356105</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B28" s="2">
+        <v>60</v>
+      </c>
+      <c r="C28" s="2">
+        <v>61.52450242224198</v>
+      </c>
+      <c r="D28" s="2">
+        <v>8</v>
+      </c>
+      <c r="F28">
+        <v>61</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="1"/>
+        <v>-0.52450242224198007</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="2"/>
+        <v>0.52450242224198007</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="4"/>
+        <v>0.27510279093770434</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" s="2">
+        <v>282</v>
+      </c>
+      <c r="C29" s="2">
+        <v>269.27694421862941</v>
+      </c>
+      <c r="D29" s="2">
+        <v>25</v>
+      </c>
+      <c r="F29">
+        <v>274</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="0"/>
+        <v>-8</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="1"/>
+        <v>4.72305578137059</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="2"/>
+        <v>4.72305578137059</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="3"/>
+        <v>64</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="4"/>
+        <v>22.307255913938153</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B30" s="2">
+        <v>19</v>
+      </c>
+      <c r="C30" s="2">
+        <v>16.209314913923421</v>
+      </c>
+      <c r="D30" s="2">
+        <v>2</v>
+      </c>
+      <c r="F30">
+        <v>16</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="1"/>
+        <v>-0.20931491392342139</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="2"/>
+        <v>0.20931491392342139</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="4"/>
+        <v>4.3812733190769303E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A31" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B31" s="2">
+        <v>791</v>
+      </c>
+      <c r="C31" s="2">
+        <v>769.31869697719685</v>
+      </c>
+      <c r="D31" s="2">
+        <v>76</v>
+      </c>
+      <c r="F31">
+        <v>810</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="1"/>
+        <v>40.681303022803149</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="2"/>
+        <v>40.681303022803149</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="3"/>
+        <v>361</v>
+      </c>
+      <c r="L31">
+        <f t="shared" si="4"/>
+        <v>1654.9684156331327</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B32" s="2">
+        <v>197</v>
+      </c>
+      <c r="C32" s="2">
+        <v>198.36803200785735</v>
+      </c>
+      <c r="D32" s="2">
+        <v>29</v>
+      </c>
+      <c r="F32">
+        <v>204</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="1"/>
+        <v>5.6319679921426484</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="2"/>
+        <v>5.6319679921426484</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="3"/>
+        <v>49</v>
+      </c>
+      <c r="L32">
+        <f t="shared" si="4"/>
+        <v>31.719063464519294</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A33" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B33" s="2">
+        <v>174</v>
+      </c>
+      <c r="C33" s="2">
+        <v>166.44721381497794</v>
+      </c>
+      <c r="D33" s="2">
+        <v>16</v>
+      </c>
+      <c r="F33">
+        <v>158</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="0"/>
+        <v>-16</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="1"/>
+        <v>-8.4472138149779425</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="2"/>
+        <v>8.4472138149779425</v>
+      </c>
+      <c r="K33">
+        <f t="shared" si="3"/>
+        <v>256</v>
+      </c>
+      <c r="L33">
+        <f t="shared" si="4"/>
+        <v>71.355421235954211</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A34" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B34" s="2">
+        <v>61</v>
+      </c>
+      <c r="C34" s="2">
+        <v>58.925734266699315</v>
+      </c>
+      <c r="D34" s="2">
+        <v>6</v>
+      </c>
+      <c r="F34">
+        <v>53</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="0"/>
+        <v>-8</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="1"/>
+        <v>-5.9257342666993154</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="2"/>
+        <v>5.9257342666993154</v>
+      </c>
+      <c r="K34">
+        <f t="shared" si="3"/>
+        <v>64</v>
+      </c>
+      <c r="L34">
+        <f t="shared" si="4"/>
+        <v>35.114326599534472</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A35" s="4" t="s">
+        <v>379</v>
+      </c>
+      <c r="B35" s="2">
+        <v>28</v>
+      </c>
+      <c r="C35" s="2">
+        <v>28.061495021629213</v>
+      </c>
+      <c r="D35" s="2">
+        <v>3</v>
+      </c>
+      <c r="F35">
+        <v>32</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="1"/>
+        <v>3.9385049783707871</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="2"/>
+        <v>3.9385049783707871</v>
+      </c>
+      <c r="K35">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="L35">
+        <f t="shared" si="4"/>
+        <v>15.511821464651474</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A36" s="4" t="s">
+        <v>428</v>
+      </c>
+      <c r="B36" s="2">
+        <v>40</v>
+      </c>
+      <c r="C36" s="2">
+        <v>40.420319507068498</v>
+      </c>
+      <c r="D36" s="2">
+        <v>2</v>
+      </c>
+      <c r="F36">
+        <v>38</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="1"/>
+        <v>-2.4203195070684984</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="2"/>
+        <v>2.4203195070684984</v>
+      </c>
+      <c r="K36">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="L36">
+        <f t="shared" si="4"/>
+        <v>5.8579465162962991</v>
+      </c>
+      <c r="M36" s="5"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A37" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B37" s="2">
         <v>1715</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C37" s="2">
         <v>1642.3864672880209</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D37" s="2">
         <v>140</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B10" s="2">
-        <v>791</v>
-      </c>
-      <c r="C10" s="2">
-        <v>769.31869697719685</v>
-      </c>
-      <c r="D10" s="2">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" s="2">
-        <v>606</v>
-      </c>
-      <c r="C11" s="2">
-        <v>595.33152670653919</v>
-      </c>
-      <c r="D11" s="2">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="B12" s="2">
-        <v>531</v>
-      </c>
-      <c r="C12" s="2">
-        <v>516.25975403563223</v>
-      </c>
-      <c r="D12" s="2">
+      <c r="F37">
+        <v>1761</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="0"/>
         <v>46</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="B13" s="2">
-        <v>505</v>
-      </c>
-      <c r="C13" s="2">
-        <v>492.0426102315655</v>
-      </c>
-      <c r="D13" s="2">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" s="2">
-        <v>465</v>
-      </c>
-      <c r="C14" s="2">
-        <v>448.35445200174451</v>
-      </c>
-      <c r="D14" s="2">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B15" s="2">
-        <v>442</v>
-      </c>
-      <c r="C15" s="2">
-        <v>431.65038303467304</v>
-      </c>
-      <c r="D15" s="2">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" s="2">
-        <v>418</v>
-      </c>
-      <c r="C16" s="2">
-        <v>406.60459841848473</v>
-      </c>
-      <c r="D16" s="2">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="B17" s="2">
-        <v>409</v>
-      </c>
-      <c r="C17" s="2">
-        <v>393.43649479845675</v>
-      </c>
-      <c r="D17" s="2">
+      <c r="H37">
+        <f t="shared" si="1"/>
+        <v>118.61353271197913</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="2"/>
+        <v>46</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="2"/>
+        <v>118.61353271197913</v>
+      </c>
+      <c r="K37">
+        <f t="shared" si="3"/>
+        <v>2116</v>
+      </c>
+      <c r="L37">
+        <f t="shared" si="4"/>
+        <v>14069.170142415744</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A38" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B38" s="2">
+        <v>256</v>
+      </c>
+      <c r="C38" s="2">
+        <v>249.147487621051</v>
+      </c>
+      <c r="D38" s="2">
+        <v>14</v>
+      </c>
+      <c r="F38">
+        <v>184</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="0"/>
+        <v>-72</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="1"/>
+        <v>-65.147487621050999</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="2"/>
+        <v>72</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="2"/>
+        <v>65.147487621050999</v>
+      </c>
+      <c r="K38">
+        <f t="shared" si="3"/>
+        <v>5184</v>
+      </c>
+      <c r="L38">
+        <f t="shared" si="4"/>
+        <v>4244.1951433349932</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A39" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B39" s="2">
         <v>30</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B18" s="2">
-        <v>362</v>
-      </c>
-      <c r="C18" s="2">
-        <v>352.16573369588434</v>
-      </c>
-      <c r="D18" s="2">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B19" s="2">
-        <v>317</v>
-      </c>
-      <c r="C19" s="2">
-        <v>307.85536265728939</v>
-      </c>
-      <c r="D19" s="2">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B20" s="2">
-        <v>302</v>
-      </c>
-      <c r="C20" s="2">
-        <v>284.34660060496839</v>
-      </c>
-      <c r="D20" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B21" s="2">
-        <v>282</v>
-      </c>
-      <c r="C21" s="2">
-        <v>269.27694421862941</v>
-      </c>
-      <c r="D21" s="2">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" s="2">
-        <v>256</v>
-      </c>
-      <c r="C22" s="2">
-        <v>249.147487621051</v>
-      </c>
-      <c r="D22" s="2">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B23" s="2">
-        <v>197</v>
-      </c>
-      <c r="C23" s="2">
-        <v>198.36803200785735</v>
-      </c>
-      <c r="D23" s="2">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B24" s="2">
-        <v>174</v>
-      </c>
-      <c r="C24" s="2">
-        <v>166.44721381497794</v>
-      </c>
-      <c r="D24" s="2">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="B25" s="2">
-        <v>121</v>
-      </c>
-      <c r="C25" s="2">
-        <v>123.42551760010409</v>
-      </c>
-      <c r="D25" s="2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B26" s="2">
-        <v>107</v>
-      </c>
-      <c r="C26" s="2">
-        <v>103.96810032766695</v>
-      </c>
-      <c r="D26" s="2">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="B27" s="2">
-        <v>88</v>
-      </c>
-      <c r="C27" s="2">
-        <v>87.099190755294501</v>
-      </c>
-      <c r="D27" s="2">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="B28" s="2">
-        <v>79</v>
-      </c>
-      <c r="C28" s="2">
-        <v>75.485696418629317</v>
-      </c>
-      <c r="D28" s="2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="B29" s="2">
-        <v>61</v>
-      </c>
-      <c r="C29" s="2">
-        <v>58.925734266699315</v>
-      </c>
-      <c r="D29" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B30" s="2">
-        <v>60</v>
-      </c>
-      <c r="C30" s="2">
-        <v>61.52450242224198</v>
-      </c>
-      <c r="D30" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="4" t="s">
-        <v>428</v>
-      </c>
-      <c r="B31" s="2">
-        <v>40</v>
-      </c>
-      <c r="C31" s="2">
-        <v>40.420319507068498</v>
-      </c>
-      <c r="D31" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="B32" s="2">
+      <c r="C39" s="2">
+        <v>28.907912798229205</v>
+      </c>
+      <c r="D39" s="2">
+        <v>4</v>
+      </c>
+      <c r="F39">
         <v>30</v>
       </c>
-      <c r="C32" s="2">
-        <v>28.907912798229205</v>
-      </c>
-      <c r="D32" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="B33" s="2">
-        <v>28</v>
-      </c>
-      <c r="C33" s="2">
-        <v>25.6571923240163</v>
-      </c>
-      <c r="D33" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="4" t="s">
-        <v>379</v>
-      </c>
-      <c r="B34" s="2">
-        <v>28</v>
-      </c>
-      <c r="C34" s="2">
-        <v>28.061495021629213</v>
-      </c>
-      <c r="D34" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="B35" s="2">
-        <v>19</v>
-      </c>
-      <c r="C35" s="2">
-        <v>16.209314913923421</v>
-      </c>
-      <c r="D35" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B36" s="2">
-        <v>13</v>
-      </c>
-      <c r="C36" s="2">
-        <v>13.015605521714182</v>
-      </c>
-      <c r="D36" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="B37" s="2">
-        <v>11</v>
-      </c>
-      <c r="C37" s="2">
-        <v>11.03313150360686</v>
-      </c>
-      <c r="D37" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="4" t="s">
-        <v>440</v>
-      </c>
-      <c r="B38" s="2">
-        <v>0</v>
-      </c>
-      <c r="C38" s="2">
-        <v>0.58402094684819805</v>
-      </c>
-      <c r="D38" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="B39" s="2">
-        <v>0</v>
-      </c>
-      <c r="C39" s="2">
-        <v>-0.33896476365591793</v>
-      </c>
-      <c r="D39" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G39">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="1"/>
+        <v>1.092087201770795</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="2"/>
+        <v>1.092087201770795</v>
+      </c>
+      <c r="K39">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L39">
+        <f t="shared" si="4"/>
+        <v>1.1926544562715651</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
         <v>586</v>
       </c>
@@ -19999,8 +20872,49 @@
       <c r="D40" s="2">
         <v>818</v>
       </c>
+      <c r="I40" s="6">
+        <f t="shared" ref="I40:J40" si="5">AVERAGE(I9:I39)</f>
+        <v>12.548387096774194</v>
+      </c>
+      <c r="J40" s="6">
+        <f t="shared" si="5"/>
+        <v>14.391144751038844</v>
+      </c>
+      <c r="K40" s="6">
+        <f>SQRT(AVERAGE(K9:K39))</f>
+        <v>19.334909094107978</v>
+      </c>
+      <c r="L40" s="6">
+        <f>SQRT(AVERAGE(L9:L39))</f>
+        <v>28.046539820416434</v>
+      </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="F9:Q37">
+    <sortCondition ref="G9:G37"/>
+  </sortState>
+  <conditionalFormatting sqref="G9:H39">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I9:J39">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>